<commit_message>
Update on cost estimation
</commit_message>
<xml_diff>
--- a/Documents/Measurement and Cost Estimation.xlsx
+++ b/Documents/Measurement and Cost Estimation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d53caa4c2cd4c0a7/SIT/Year 2/Year 2 Tri 3/OIP/Repo/OIPTeam27/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="8_{D10B7C98-4FAF-48A5-A359-EAACD7ED20D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49247D53-5DE7-4150-AFEF-7EF4E2E7AA0C}"/>
+  <xr:revisionPtr revIDLastSave="153" documentId="8_{D10B7C98-4FAF-48A5-A359-EAACD7ED20D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7AF5158-7749-4761-B395-64A823509AE3}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1590" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6D16CCE7-B2FF-4158-84F8-5DAF7E7D6598}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{6D16CCE7-B2FF-4158-84F8-5DAF7E7D6598}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>length</t>
   </si>
@@ -76,18 +76,12 @@
     <t>Touch Screen</t>
   </si>
   <si>
-    <t xml:space="preserve">Misc </t>
-  </si>
-  <si>
     <t>Raspberry Pi Zero WH (with Header)</t>
   </si>
   <si>
     <t>Heated Hair Dryer</t>
   </si>
   <si>
-    <t>Camera 8MP V2</t>
-  </si>
-  <si>
     <t>Per Syringe</t>
   </si>
   <si>
@@ -155,6 +149,9 @@
   </si>
   <si>
     <t>Overall estimated dimension (337 x 105 x 360mm)</t>
+  </si>
+  <si>
+    <t>Infrared Sensor</t>
   </si>
 </sst>
 </file>
@@ -575,21 +572,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D5F0AF-5DF3-4434-901A-ADDDA6FEB033}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.3984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
@@ -603,7 +600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -617,13 +614,13 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2">
         <v>24.14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -637,13 +634,13 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3">
         <v>6.21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -663,134 +660,114 @@
         <v>2.56</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>41.07</v>
+        <v>9.9</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G5">
-        <v>15.96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>9.9</v>
+        <v>5</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G6">
-        <v>1.58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>4.9400000000000004</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4.9400000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>4.9400000000000004</v>
+        <v>63</v>
       </c>
       <c r="E8">
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8">
-        <v>4.9400000000000004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C9">
-        <v>16.8</v>
+        <v>18.95</v>
       </c>
       <c r="E9">
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="G9">
-        <v>12.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
+        <v>18.95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C10">
-        <v>42.63</v>
-      </c>
-      <c r="E10">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>13</v>
+        <f>SUM(C2:C9)</f>
+        <v>181.45</v>
       </c>
       <c r="G10">
-        <v>42.63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <f>SUM(C2:C10)</f>
-        <v>200</v>
-      </c>
-      <c r="G11">
-        <f>SUM(G2:G10)</f>
-        <v>115.82</v>
+        <f>SUM(G2:G9)</f>
+        <v>105.38000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -803,32 +780,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B5CDEA0-00AF-4ECE-8294-BABF3320F42B}">
   <dimension ref="A2:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -836,7 +813,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -844,7 +821,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -852,73 +829,73 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>90</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11">
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E12">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E13">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>15</v>
@@ -930,37 +907,37 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E15">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E16">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>6</v>
@@ -970,37 +947,37 @@
         <v>360</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B19">
         <f>SUM(B11:B18)</f>
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
@@ -1009,23 +986,23 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>76</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E23">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B24">
         <v>20</v>
@@ -1035,44 +1012,44 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B25">
         <f>B23+B24</f>
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B28">
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>96</v>
       </c>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B30">
         <f>B28+B29</f>
         <v>337</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>